<commit_message>
Jogo de Campo Minado 20/08
</commit_message>
<xml_diff>
--- a/Aula-Python-12-08/campo.xlsx
+++ b/Aula-Python-12-08/campo.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -30,12 +30,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
       <sz val="11"/>
     </font>
   </fonts>
@@ -66,25 +60,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
@@ -480,43 +468,43 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
-      <c r="A1" s="7" t="inlineStr">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>linhas</t>
         </is>
       </c>
-      <c r="B1" s="7" t="inlineStr">
-        <is>
-          <t>5</t>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1">
-      <c r="A2" s="7" t="inlineStr">
+      <c r="A2" s="5" t="inlineStr">
         <is>
           <t>colunas</t>
         </is>
       </c>
-      <c r="B2" s="7" t="inlineStr">
-        <is>
-          <t>5</t>
+      <c r="B2" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="3" ht="18.75" customHeight="1">
-      <c r="A3" s="7" t="inlineStr">
+      <c r="A3" s="5" t="inlineStr">
         <is>
           <t>dificuldade</t>
         </is>
       </c>
-      <c r="B3" s="7" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="B3" s="4" t="inlineStr">
+        <is>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -531,7 +519,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -539,96 +527,35 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="3" max="3"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="5" max="5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1">
-      <c r="A1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="n">
-        <v>-2</v>
-      </c>
-      <c r="C1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="n">
-        <v>-1</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
-    <row r="2" ht="19.5" customHeight="1">
-      <c r="A2" s="1" t="n">
-        <v>-1</v>
-      </c>
-      <c r="B2" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" s="5" t="n">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="3" ht="19.5" customHeight="1">
-      <c r="A3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="B3" s="5" t="n">
-        <v>-2</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="5" t="n">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="4" ht="19.5" customHeight="1">
-      <c r="A4" s="1" t="n">
-        <v>-1</v>
-      </c>
-      <c r="B4" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E4" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" ht="18.75" customHeight="1">
-      <c r="A5" s="1" t="n">
-        <v>-1</v>
-      </c>
-      <c r="B5" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="5" t="n">
-        <v>-1</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>